<commit_message>
update to also include PdeltaAIC as a cov for CG path
</commit_message>
<xml_diff>
--- a/tables/Heterogen_MetaAnalyses_Precipitation.xlsx
+++ b/tables/Heterogen_MetaAnalyses_Precipitation.xlsx
@@ -59,10 +59,10 @@
     <t xml:space="preserve">ZG</t>
   </si>
   <si>
-    <t xml:space="preserve"> 201.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.445</t>
+    <t xml:space="preserve"> 195.9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.429</t>
   </si>
   <si>
     <t xml:space="preserve">CG</t>
@@ -77,7 +77,7 @@
     <t xml:space="preserve">PG</t>
   </si>
   <si>
-    <t xml:space="preserve"> 111.8</t>
+    <t xml:space="preserve"> 112.3</t>
   </si>
   <si>
     <t xml:space="preserve">0.000</t>
@@ -86,19 +86,19 @@
     <t xml:space="preserve">CZG</t>
   </si>
   <si>
-    <t xml:space="preserve">0.486</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 153.9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.350</t>
+    <t xml:space="preserve">0.473</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 153.6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.351</t>
   </si>
   <si>
     <t xml:space="preserve">TotalCG</t>
   </si>
   <si>
-    <t xml:space="preserve">0.005</t>
+    <t xml:space="preserve">0.006</t>
   </si>
   <si>
     <t xml:space="preserve">1629.1</t>
@@ -116,10 +116,10 @@
     <t xml:space="preserve">0.528</t>
   </si>
   <si>
-    <t xml:space="preserve"> 137.5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.369</t>
+    <t xml:space="preserve"> 136.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.415</t>
   </si>
   <si>
     <t xml:space="preserve">0.002</t>
@@ -131,16 +131,16 @@
     <t xml:space="preserve">0.680</t>
   </si>
   <si>
-    <t xml:space="preserve"> 101.8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.060</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.227</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  58.7</t>
+    <t xml:space="preserve"> 101.9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.059</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.224</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  58.6</t>
   </si>
   <si>
     <t xml:space="preserve">0.997</t>

</xml_diff>